<commit_message>
Added check for valid EAN. Changed order of columns in excel template.
</commit_message>
<xml_diff>
--- a/Presentation.Web/Content/excel/OS2KITOS Organisationsenheder.xlsx
+++ b/Presentation.Web/Content/excel/OS2KITOS Organisationsenheder.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Organisationsenheder" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Afdelingsnavne" localSheetId="0">Organisationsenheder!$B$2:$B$1000</definedName>
+    <definedName name="Afdelingsnavne" localSheetId="0">Organisationsenheder!$C$2:$C$1000</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -132,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -140,6 +140,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -481,16 +485,15 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="6" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="4" bestFit="1" customWidth="1"/>
@@ -504,13 +507,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -519,12 +522,12 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0"/>
   <dataValidations count="2">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:J1048576">
       <formula1>29221</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
       <formula1>Afdelingsnavne</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>